<commit_message>
runoff grid catchment intersect calculated in arc
</commit_message>
<xml_diff>
--- a/1_Data/GIS_data/runoff_grid_catchment_intrsct.xlsx
+++ b/1_Data/GIS_data/runoff_grid_catchment_intrsct.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masters\Thesis\1_Data\GIS_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C73724-FC77-4F06-8867-59E055E3B202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009110A8-E1B6-40D4-A9EF-F86F36BA14D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,16 +194,13 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -211,6 +208,9 @@
           <color rgb="FF000000"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -226,17 +226,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E061146B-A951-4DDC-B5D2-A1353A4CD1BA}" name="Table1" displayName="Table1" ref="A1:I30" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4" headerRowCellStyle="Style0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E061146B-A951-4DDC-B5D2-A1353A4CD1BA}" name="Table1" displayName="Table1" ref="A1:I30" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" headerRowCellStyle="Style0">
   <autoFilter ref="A1:I30" xr:uid="{E061146B-A951-4DDC-B5D2-A1353A4CD1BA}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7A2EA570-F7EB-4F84-B84C-B6CC8C36FAB9}" name="OBJECTID"/>
     <tableColumn id="2" xr3:uid="{255E02AB-9CD5-450F-AA6A-3CF2DCEB5BF1}" name="OBJECTID2"/>
     <tableColumn id="7" xr3:uid="{B3FA644E-9642-4A47-BB4F-A87A8AE10BAE}" name="Input_FID"/>
     <tableColumn id="3" xr3:uid="{F2CF2966-A4D8-49F1-9B0E-2DC6151B5ABF}" name="Name"/>
-    <tableColumn id="8" xr3:uid="{6CEBC1FC-C88F-4B47-AF9B-9244487DD9F4}" name="lat" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{1C322865-6E4F-490F-B3A8-BE013FD4605C}" name="lon" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{6CEBC1FC-C88F-4B47-AF9B-9244487DD9F4}" name="lat" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{1C322865-6E4F-490F-B3A8-BE013FD4605C}" name="lon" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{6BCDADED-C657-4246-A757-FEE046C2C141}" name="intersect_AREA"/>
-    <tableColumn id="5" xr3:uid="{355B950F-8131-455B-B074-3FB704B03042}" name="%_overlap" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{355B950F-8131-455B-B074-3FB704B03042}" name="%_overlap" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{2DD52610-CC22-4FA1-8597-2E04B69D5619}" name="geod_area"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>